<commit_message>
corrected date form 01.16.19 to 01.16.20
</commit_message>
<xml_diff>
--- a/library/Library_hbrown_01.16.20.xlsx
+++ b/library/Library_hbrown_01.16.20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538B94E2-D865-D345-8E9A-4E6B9B0BC017}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB9E0C8-7273-0F46-AF67-C5A5FE85DFB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="3740" windowWidth="27640" windowHeight="12740" xr2:uid="{1EA5AFFF-1344-0B40-9643-C4B9123AC6F1}"/>
+    <workbookView xWindow="1280" yWindow="1520" windowWidth="13640" windowHeight="12740" xr2:uid="{1EA5AFFF-1344-0B40-9643-C4B9123AC6F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>roboticLibraryPrep</t>
   </si>
   <si>
-    <t>01.16.19</t>
-  </si>
-  <si>
     <t>H.BROWN</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>TCCGGGA</t>
+  </si>
+  <si>
+    <t>01.16.20</t>
   </si>
 </sst>
 </file>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DB408A0-6804-574E-BFA8-61CA29FA5D78}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -594,19 +594,19 @@
     </row>
     <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -615,36 +615,36 @@
         <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -653,36 +653,36 @@
         <v>28</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -691,36 +691,36 @@
         <v>29</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -729,36 +729,36 @@
         <v>30</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -767,36 +767,36 @@
         <v>31</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -805,36 +805,36 @@
         <v>32</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8">
         <v>7</v>
@@ -843,36 +843,36 @@
         <v>33</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9">
         <v>8</v>
@@ -881,36 +881,36 @@
         <v>34</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10">
         <v>9</v>
@@ -919,36 +919,36 @@
         <v>35</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11">
         <v>10</v>
@@ -957,36 +957,36 @@
         <v>36</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F12">
         <v>11</v>
@@ -995,36 +995,36 @@
         <v>37</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13">
         <v>12</v>
@@ -1033,36 +1033,36 @@
         <v>38</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14">
         <v>13</v>
@@ -1071,36 +1071,36 @@
         <v>39</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15">
         <v>14</v>
@@ -1109,36 +1109,36 @@
         <v>40</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F16">
         <v>15</v>
@@ -1147,36 +1147,36 @@
         <v>41</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F17">
         <v>16</v>
@@ -1185,36 +1185,36 @@
         <v>42</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F18">
         <v>17</v>
@@ -1223,36 +1223,36 @@
         <v>43</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F19">
         <v>18</v>
@@ -1261,36 +1261,36 @@
         <v>44</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20">
         <v>19</v>
@@ -1299,36 +1299,36 @@
         <v>45</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F21">
         <v>20</v>
@@ -1337,36 +1337,36 @@
         <v>46</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F22">
         <v>21</v>
@@ -1375,36 +1375,36 @@
         <v>47</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23">
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F23">
         <v>22</v>
@@ -1413,36 +1413,36 @@
         <v>48</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24">
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F24">
         <v>23</v>
@@ -1451,36 +1451,36 @@
         <v>49</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25">
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F25">
         <v>24</v>
@@ -1489,36 +1489,36 @@
         <v>50</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26">
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F26">
         <v>25</v>
@@ -1527,36 +1527,36 @@
         <v>51</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F27">
         <v>26</v>
@@ -1565,36 +1565,36 @@
         <v>52</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C28">
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F28">
         <v>27</v>
@@ -1603,36 +1603,36 @@
         <v>53</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C29">
         <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F29">
         <v>28</v>
@@ -1641,36 +1641,36 @@
         <v>54</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C30">
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F30">
         <v>29</v>
@@ -1679,36 +1679,36 @@
         <v>55</v>
       </c>
       <c r="H30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C31">
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F31">
         <v>30</v>
@@ -1717,36 +1717,36 @@
         <v>56</v>
       </c>
       <c r="H31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C32">
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F32">
         <v>31</v>
@@ -1755,19 +1755,19 @@
         <v>57</v>
       </c>
       <c r="H32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>